<commit_message>
Suppression des contacts dans les états : Etat trimestriel collectivité CS, Etat mensuel collectivité HCS, Etat mensuel des réceptions, Fiche de répartition. Possibilité d'avoir plusieurs contacts "e-mailing NDC CL". Envoi des e-mails NDC à tous les contacts : modification structures BDD et objets métiers, modification de l'envoi en masse. Possibilité d'imprimer, en masse ou à l'unité, les certificats de recyclage et les états mensuels HCS CL. Revue du design des modèles Excel pour un meilleur affichage quel que soit la taille du nom de la collectivité
</commit_message>
<xml_diff>
--- a/eVaSys.Server/Assets/Templates/CertificatRecyclage.xlsx
+++ b/eVaSys.Server/Assets/Templates/CertificatRecyclage.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\Repos\Valorplast\eValorplastWebApp\Assets\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\Repos\eVaSys\eVaSys.Server\Assets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54C37F8-EC76-4F4D-957B-D62D92BF7972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C641193-508B-4D94-90CF-EFBBEBFB02D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5532" yWindow="3456" windowWidth="22776" windowHeight="19788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6288" yWindow="3924" windowWidth="20736" windowHeight="18912" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certificat" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -273,13 +273,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>1857375</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -324,15 +324,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>617683</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:colOff>536600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>236220</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -361,8 +361,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1905463" cy="1074420"/>
+          <a:off x="1" y="0"/>
+          <a:ext cx="1824379" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -620,63 +620,63 @@
     <col min="8" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" ht="21" x14ac:dyDescent="0.4">
       <c r="C4" s="3"/>
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="3:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" ht="21" x14ac:dyDescent="0.4">
       <c r="C5" s="3"/>
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
-      <c r="E9" s="10" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="D9" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
-      <c r="E10" s="10" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="D10" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
-      <c r="E11" s="10" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="D11" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="8" t="s">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="9" t="s">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>